<commit_message>
feat: automation safepoint && query data retrieving fix
</commit_message>
<xml_diff>
--- a/data_with_all_devices.xlsx
+++ b/data_with_all_devices.xlsx
@@ -7958,7 +7958,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7968,13 +7968,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -8032,10 +8026,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -8362,7 +8356,7 @@
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8388,7 +8382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -8414,7 +8408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -8440,7 +8434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -8466,7 +8460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -8492,7 +8486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -8518,7 +8512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -8544,7 +8538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -8570,7 +8564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -8596,7 +8590,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -8622,7 +8616,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -8648,7 +8642,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -8674,7 +8668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -8700,7 +8694,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -8726,7 +8720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>